<commit_message>
Updated names in folders and 'sections.xlsx' sample
</commit_message>
<xml_diff>
--- a/sections-spring-2026.xlsx
+++ b/sections-spring-2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Stephen/Desktop/ZLP_DEMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F35B22-6053-9247-9E65-37041EF7C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B784D6-6EA4-3E45-837A-AAED894A6D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,8 +540,8 @@
   </sheetPr>
   <dimension ref="A1:Z1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:I131"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>